<commit_message>
got hamming distance for c3540
</commit_message>
<xml_diff>
--- a/c3540/c880 and c3540 io.xlsx
+++ b/c3540/c880 and c3540 io.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/TheFolder/Documents/ECE 459/Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jtvar\ECE459\Project\ECE459PUF-Maker\c3540\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{887CD723-C713-654D-A1D2-362DB049DEC2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E4ADEC3-934D-427E-97AE-54C7131C58CC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="14760" xr2:uid="{0905E3DD-815B-2B4C-A5D9-53817CD19009}"/>
+    <workbookView xWindow="20370" yWindow="-9015" windowWidth="29040" windowHeight="16440" xr2:uid="{0905E3DD-815B-2B4C-A5D9-53817CD19009}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
   <si>
     <t>C3540</t>
   </si>
@@ -184,6 +184,12 @@
   </si>
   <si>
     <t>00010111101000110101000100</t>
+  </si>
+  <si>
+    <t>Random Keys</t>
+  </si>
+  <si>
+    <t>correct key</t>
   </si>
 </sst>
 </file>
@@ -536,29 +542,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{347F5D6A-048F-8D41-B15C-C4584D1C6AF9}">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="56" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="62.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="62.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -571,8 +580,11 @@
       <c r="E2" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G2">
+        <v>101101111</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -585,8 +597,11 @@
       <c r="E3" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G3">
+        <v>100110001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -599,8 +614,11 @@
       <c r="E4" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G4">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -613,8 +631,11 @@
       <c r="E5" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G5">
+        <v>111101011</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
@@ -627,8 +648,11 @@
       <c r="E6" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G6">
+        <v>101001111</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
@@ -641,8 +665,11 @@
       <c r="E7" s="1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G7">
+        <v>101000010</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
@@ -655,8 +682,11 @@
       <c r="E8" s="1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G8">
+        <v>1011111</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>15</v>
       </c>
@@ -669,8 +699,11 @@
       <c r="E9" s="1" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G9">
+        <v>1100100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>17</v>
       </c>
@@ -683,8 +716,11 @@
       <c r="E10" s="1" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G10">
+        <v>101100010</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>19</v>
       </c>
@@ -697,8 +733,11 @@
       <c r="E11" s="1" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G11">
+        <v>11001101</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>21</v>
       </c>
@@ -711,8 +750,11 @@
       <c r="E12" s="1" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G12">
+        <v>110010001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>23</v>
       </c>
@@ -724,6 +766,17 @@
       </c>
       <c r="E13" s="1" t="s">
         <v>49</v>
+      </c>
+      <c r="G13">
+        <v>10010101</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E14" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F14">
+        <v>110100100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>